<commit_message>
update slurry comp inputs
</commit_message>
<xml_diff>
--- a/emis_preds/inputs/inputs.xlsx
+++ b/emis_preds/inputs/inputs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sasha\Git-repos\Pedersen-2022-app-digestate-NH3-review\emis_preds\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E802B66E-D2D0-46ED-9319-FFD426E68CEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B029428B-B5D8-46EE-AF27-35C278D95834}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="375" yWindow="8520" windowWidth="7500" windowHeight="1140" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Slurry" sheetId="1" r:id="rId1"/>
@@ -38,35 +38,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="37">
   <si>
     <t>man.source</t>
   </si>
   <si>
-    <t>acid</t>
-  </si>
-  <si>
     <t>man.dm</t>
   </si>
   <si>
     <t>man.ph</t>
   </si>
   <si>
-    <t>Svinegylle</t>
-  </si>
-  <si>
-    <t>FALSE</t>
-  </si>
-  <si>
-    <t>Kvæggylle</t>
-  </si>
-  <si>
-    <t>Afgasset biomasse</t>
-  </si>
-  <si>
-    <t>TRUE</t>
-  </si>
-  <si>
     <t>app.timing</t>
   </si>
   <si>
@@ -122,6 +104,51 @@
   </si>
   <si>
     <t>Update!</t>
+  </si>
+  <si>
+    <t>man.descrip</t>
+  </si>
+  <si>
+    <t>pig EF report</t>
+  </si>
+  <si>
+    <t>cattle EF report</t>
+  </si>
+  <si>
+    <t>digestate EF report</t>
+  </si>
+  <si>
+    <t>Pig</t>
+  </si>
+  <si>
+    <t>Cattle</t>
+  </si>
+  <si>
+    <t>Digestate A</t>
+  </si>
+  <si>
+    <t>Digestate B</t>
+  </si>
+  <si>
+    <t>digestate cris</t>
+  </si>
+  <si>
+    <t>digestate cattle lit</t>
+  </si>
+  <si>
+    <t>Digestate CL</t>
+  </si>
+  <si>
+    <t>Digestate PL</t>
+  </si>
+  <si>
+    <t>digestate pig lit</t>
+  </si>
+  <si>
+    <t>digestate mix lit</t>
+  </si>
+  <si>
+    <t>Digestate ML</t>
   </si>
 </sst>
 </file>
@@ -131,16 +158,10 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
-      <name val="Sans"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF3465A4"/>
       <name val="Sans"/>
       <charset val="1"/>
     </font>
@@ -165,18 +186,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -556,7 +571,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -564,123 +579,129 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AMI9"/>
+  <dimension ref="A1:AMI8"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.140625" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="16.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" style="2"/>
+    <col min="1" max="1" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" style="1" customWidth="1"/>
     <col min="3" max="1023" width="10.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>26</v>
       </c>
       <c r="C2" s="1">
         <v>3.9</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="2">
         <v>7.2</v>
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>5</v>
+      <c r="A3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>27</v>
       </c>
       <c r="C3" s="1">
         <v>6.5</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="2">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>5</v>
+      <c r="A4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>28</v>
       </c>
       <c r="C4" s="1">
         <v>5.9</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="2">
         <v>7.9</v>
       </c>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="2" t="s">
+      <c r="A5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" s="1">
+        <v>7.2</v>
+      </c>
+      <c r="D5" s="2">
         <v>8</v>
       </c>
-      <c r="C5" s="1">
-        <v>3.9</v>
-      </c>
-      <c r="D5" s="4">
-        <f>D2-0.73</f>
-        <v>6.4700000000000006</v>
-      </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>8</v>
+      <c r="A6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="C6" s="1">
-        <v>6.5</v>
-      </c>
-      <c r="D6" s="4">
-        <f>D3-0.53</f>
-        <v>6.47</v>
+        <v>4.03</v>
+      </c>
+      <c r="D6" s="2">
+        <v>7.33</v>
       </c>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>8</v>
+      <c r="A7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="C7" s="1">
-        <v>5.9</v>
-      </c>
-      <c r="D7" s="4">
-        <f>D4-1.38</f>
-        <v>6.5200000000000005</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" s="1" t="s">
-        <v>27</v>
+        <v>3.68</v>
+      </c>
+      <c r="D7" s="2">
+        <v>7.67</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" s="2">
+        <v>4.55</v>
+      </c>
+      <c r="D8" s="2">
+        <v>8.16</v>
       </c>
     </row>
   </sheetData>
@@ -712,91 +733,91 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="5">
+        <v>7</v>
+      </c>
+      <c r="B2" s="3">
         <v>4.43101207056639</v>
       </c>
-      <c r="C2" s="5">
+      <c r="C2" s="3">
         <v>4.05891613991413</v>
       </c>
-      <c r="D2" s="5">
+      <c r="D2" s="3">
         <v>5.99629009095261E-2</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="5">
+        <v>8</v>
+      </c>
+      <c r="B3" s="3">
         <v>8.23645983645984</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="3">
         <v>3.8444559186574501</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="3">
         <v>5.5211941283193101E-2</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" s="5">
+        <v>9</v>
+      </c>
+      <c r="B4" s="3">
         <v>12.4492495309568</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="3">
         <v>3.4839152629563301</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="3">
         <v>7.0299348896299796E-2</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="5">
+        <v>10</v>
+      </c>
+      <c r="B5" s="3">
         <v>16.876225981619299</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="3">
         <v>3.1562401242322702</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="3">
         <v>0.105925308296069</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" s="5">
+        <v>11</v>
+      </c>
+      <c r="B6" s="3">
         <v>14.4977479635841</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="3">
         <v>3.3227695983363299</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="3">
         <v>0.12826017044540899</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -813,7 +834,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AMI8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
@@ -825,24 +846,24 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="D2" s="1">
         <v>30</v>
@@ -850,10 +871,10 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="1" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C3" s="1">
         <v>4</v>
@@ -864,10 +885,10 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="1" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="D4" s="1">
         <v>0</v>
@@ -875,10 +896,10 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="1" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="D5" s="1">
         <v>0</v>
@@ -886,7 +907,7 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add mean calc, add new summ stats to plot, A, B, C
</commit_message>
<xml_diff>
--- a/emis_preds/inputs/inputs.xlsx
+++ b/emis_preds/inputs/inputs.xlsx
@@ -60,24 +60,6 @@
     <t xml:space="preserve">Digestate B</t>
   </si>
   <si>
-    <t xml:space="preserve">digestate cattle lit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Digestate CL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">digestate pig lit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Digestate PL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">digestate mix lit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Digestate ML</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <sz val="10"/>
@@ -101,7 +83,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Digestate low</t>
+    <t xml:space="preserve">Digestate B low</t>
   </si>
   <si>
     <r>
@@ -127,7 +109,65 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Digestate high</t>
+    <t xml:space="preserve">Digestate B high</t>
+  </si>
+  <si>
+    <t xml:space="preserve">digestate lit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Digestate C</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Sans"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">digestate lit 10</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Sans"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">th</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Digestate C low</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Sans"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">digestate lit 90</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Sans"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">th</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Digestate C high</t>
   </si>
   <si>
     <t xml:space="preserve">app.timing</t>
@@ -292,17 +332,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
+      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.14453125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.12890625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="16.86"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1023" min="3" style="1" width="10.14"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1023" min="3" style="1" width="10.13"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -383,10 +423,10 @@
         <v>13</v>
       </c>
       <c r="C6" s="1" t="n">
-        <v>4.03</v>
-      </c>
-      <c r="D6" s="2" t="n">
-        <v>7.33</v>
+        <v>5.45</v>
+      </c>
+      <c r="D6" s="1" t="n">
+        <v>7.864</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -397,10 +437,10 @@
         <v>15</v>
       </c>
       <c r="C7" s="1" t="n">
-        <v>3.68</v>
-      </c>
-      <c r="D7" s="2" t="n">
-        <v>7.67</v>
+        <v>9.114</v>
+      </c>
+      <c r="D7" s="1" t="n">
+        <v>8.282</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -410,11 +450,11 @@
       <c r="B8" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="2" t="n">
-        <v>4.55</v>
-      </c>
-      <c r="D8" s="2" t="n">
-        <v>8.16</v>
+      <c r="C8" s="1" t="n">
+        <v>3.87</v>
+      </c>
+      <c r="D8" s="1" t="n">
+        <v>7.97</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -425,10 +465,10 @@
         <v>19</v>
       </c>
       <c r="C9" s="1" t="n">
-        <v>5.45</v>
-      </c>
-      <c r="D9" s="1" t="n">
-        <v>7.864</v>
+        <v>1.99</v>
+      </c>
+      <c r="D9" s="2" t="n">
+        <v>7.41</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -439,12 +479,19 @@
         <v>21</v>
       </c>
       <c r="C10" s="1" t="n">
-        <v>9.114</v>
-      </c>
-      <c r="D10" s="1" t="n">
-        <v>8.282</v>
-      </c>
-    </row>
+        <v>5.54</v>
+      </c>
+      <c r="D10" s="2" t="n">
+        <v>8.53</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+    </row>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -467,13 +514,13 @@
       <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.14453125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.12890625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="8.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="8.29"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1023" min="5" style="1" width="10.14"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1023" min="5" style="1" width="10.13"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -582,10 +629,10 @@
       <selection pane="topLeft" activeCell="C23" activeCellId="0" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.14453125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.12890625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="17.29"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1023" min="2" style="1" width="10.14"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1023" min="2" style="1" width="10.13"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>